<commit_message>
fixed the excel file into csv
</commit_message>
<xml_diff>
--- a/test_csvs/assignments/Lin_Assignment.xlsx
+++ b/test_csvs/assignments/Lin_Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\46783590\Desktop\BoxSyncSMU\Box Sync\5330f20\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayharper/Desktop/SMU/Grad School/2nd_semester/file_org/final_project_group/test_csvs/assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F9D6067-C954-43CC-89FA-C8ED3DBB231C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CE2074-67B3-C44D-9B1C-722285BA4F59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{828AFEBF-5821-4C5A-9AEF-98B5B3F8E0C0}"/>
+    <workbookView xWindow="1160" yWindow="2720" windowWidth="27680" windowHeight="13520" xr2:uid="{828AFEBF-5821-4C5A-9AEF-98B5B3F8E0C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,13 +426,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06C60BC-3BC4-4747-85F6-B3E1F5578FCC}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -465,7 +465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -498,7 +498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -509,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -542,7 +542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -553,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -575,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -586,7 +586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -597,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -608,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -619,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -630,7 +630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -641,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -652,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -663,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -685,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -696,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -707,7 +707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -718,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -729,7 +729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>12</v>
       </c>

</xml_diff>